<commit_message>
@Xantam Update to Map032 scene update
</commit_message>
<xml_diff>
--- a/data/Actors.xlsx
+++ b/data/Actors.xlsx
@@ -462,7 +462,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,179 +470,179 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" t="s">
         <v>28</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Updated translation patch to support the huge v2 update.
</commit_message>
<xml_diff>
--- a/data/Actors.xlsx
+++ b/data/Actors.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>アルス</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>ウォルフ</t>
+  </si>
+  <si>
+    <t>リリー</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,181 +473,273 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="D21" t="s">
+      <c r="B21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26" t="s">
         <v>28</v>
       </c>
-      <c r="D26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>